<commit_message>
post process of Excel- bullets, merge cells
</commit_message>
<xml_diff>
--- a/src/docs/SampleTable.xlsx
+++ b/src/docs/SampleTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dctlchn\src\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6BF4E9C-8064-4F35-9E75-855C888C7919}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C24B8619-83DD-4F62-9D2C-7ABE8458543F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{52CCC0D4-432A-4BEC-84E5-9AE94DB33649}"/>
   </bookViews>
@@ -1973,7 +1973,7 @@
   <dimension ref="A1:D93"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25:C27"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
retry of Excel export with original file
</commit_message>
<xml_diff>
--- a/src/docs/SampleTable.xlsx
+++ b/src/docs/SampleTable.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dctlchn\src\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AbaStuff\IZDocsGitHub\AAGit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C24B8619-83DD-4F62-9D2C-7ABE8458543F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B09BF35B-2B75-49DB-B2AD-FD2220C5EDD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{52CCC0D4-432A-4BEC-84E5-9AE94DB33649}"/>
+    <workbookView xWindow="4800" yWindow="2800" windowWidth="14400" windowHeight="7400" xr2:uid="{52CCC0D4-432A-4BEC-84E5-9AE94DB33649}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="140">
   <si>
     <t>Item</t>
   </si>
@@ -120,6 +120,81 @@
     <t>Up to 120 mph (193 km/h)</t>
   </si>
   <si>
+    <t>LPR Capture Distance*</t>
+  </si>
+  <si>
+    <t>(for U.S.A. plates)</t>
+  </si>
+  <si>
+    <r>
+      <t>n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>G/GW-S-XX – 16-39 ft (5-12 m)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>G/GW-L-XX – 33-65 ft (10-20 m)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>G/GW-XL-XX – 33-80 ft (10-24 m)</t>
+    </r>
+  </si>
+  <si>
     <t>LPR Illumination</t>
   </si>
   <si>
@@ -1100,42 +1175,13 @@
   </si>
   <si>
     <t>External Illuminator (IZS Series)</t>
-  </si>
-  <si>
-    <t>LPR Capture Distance* (for U.S.A. plates)</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9.5"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>* G/GW-S-XX – 16-39 ft (5-12 m)
-* G/GW-L-XX – 33-65 ft (10-20 m)
-* G/GW-XL-XX – 33-80 ft (10-24 m)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8.5"/>
-        <color theme="1"/>
-        <rFont val="Wingdings"/>
-        <charset val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-  </si>
-  <si>
-    <t>* G-S-XX – 12-40 mm; Motorized Zoom and Auto-focus</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1195,13 +1241,6 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="8.5"/>
-      <color theme="1"/>
-      <name val="Wingdings"/>
-      <family val="2"/>
-      <charset val="2"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1480,7 +1519,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1509,152 +1548,149 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1972,8 +2008,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBB5F46E-3BC1-4BB0-BA5A-3AD2C390191A}">
   <dimension ref="A1:D93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1985,10 +2021,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="49"/>
+      <c r="B1" s="11"/>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1997,10 +2033,10 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="36"/>
+      <c r="B2" s="13"/>
       <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
@@ -2009,902 +2045,996 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="19"/>
+      <c r="D3" s="20"/>
     </row>
     <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="25"/>
-      <c r="B4" s="25"/>
-      <c r="C4" s="18" t="s">
+      <c r="A4" s="14"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="19"/>
+      <c r="D4" s="20"/>
     </row>
     <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="25"/>
-      <c r="B5" s="26"/>
-      <c r="C5" s="18" t="s">
+      <c r="A5" s="14"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="19"/>
+      <c r="D5" s="20"/>
     </row>
     <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="25"/>
-      <c r="B6" s="22" t="s">
+      <c r="A6" s="14"/>
+      <c r="B6" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="19"/>
+      <c r="D6" s="20"/>
     </row>
     <row r="7" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="25"/>
-      <c r="B7" s="25"/>
-      <c r="C7" s="18" t="s">
+      <c r="A7" s="14"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="19"/>
+      <c r="D7" s="20"/>
     </row>
     <row r="8" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="25"/>
-      <c r="B8" s="25"/>
-      <c r="C8" s="18" t="s">
+      <c r="A8" s="14"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="19"/>
+      <c r="D8" s="20"/>
     </row>
     <row r="9" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="23"/>
-      <c r="B9" s="23"/>
-      <c r="C9" s="20" t="s">
+      <c r="A9" s="16"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="21"/>
+      <c r="D9" s="22"/>
     </row>
     <row r="10" spans="1:4" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="44" t="s">
+      <c r="A10" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="45"/>
-      <c r="C10" s="46" t="s">
+      <c r="B10" s="25"/>
+      <c r="C10" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="47"/>
+      <c r="D10" s="27"/>
     </row>
     <row r="11" spans="1:4" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="44" t="s">
+      <c r="A11" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="45"/>
-      <c r="C11" s="46" t="s">
+      <c r="B11" s="25"/>
+      <c r="C11" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="47"/>
+      <c r="D11" s="27"/>
     </row>
     <row r="12" spans="1:4" ht="24" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="30"/>
+      <c r="C12" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="34"/>
+    </row>
+    <row r="13" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="17"/>
+      <c r="C13" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="36"/>
+    </row>
+    <row r="14" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="31"/>
+      <c r="B14" s="32"/>
+      <c r="C14" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="38"/>
+    </row>
+    <row r="15" spans="1:4" ht="84.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="48" x14ac:dyDescent="0.35">
+      <c r="A16" s="14"/>
+      <c r="B16" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="48" x14ac:dyDescent="0.35">
+      <c r="A17" s="14"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="60.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="14"/>
+      <c r="B18" s="18"/>
+      <c r="C18" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="48" x14ac:dyDescent="0.35">
+      <c r="A19" s="14"/>
+      <c r="B19" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="48" x14ac:dyDescent="0.35">
+      <c r="A20" s="14"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="60.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="16"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" s="40" t="s">
+        <v>44</v>
+      </c>
+      <c r="D22" s="41"/>
+    </row>
+    <row r="23" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="14"/>
+      <c r="B23" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="D23" s="43"/>
+    </row>
+    <row r="24" spans="1:4" ht="24.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="14"/>
+      <c r="B24" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="D24" s="20"/>
+    </row>
+    <row r="25" spans="1:4" ht="48" x14ac:dyDescent="0.35">
+      <c r="A25" s="14"/>
+      <c r="B25" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="36" x14ac:dyDescent="0.35">
+      <c r="A26" s="14"/>
+      <c r="B26" s="14"/>
+      <c r="C26" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="24" x14ac:dyDescent="0.35">
+      <c r="A27" s="14"/>
+      <c r="B27" s="14"/>
+      <c r="C27" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="48" x14ac:dyDescent="0.35">
+      <c r="A28" s="14"/>
+      <c r="B28" s="14"/>
+      <c r="C28" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="36" x14ac:dyDescent="0.35">
+      <c r="A29" s="14"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="24" x14ac:dyDescent="0.35">
+      <c r="A30" s="14"/>
+      <c r="B30" s="14"/>
+      <c r="C30" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="48" x14ac:dyDescent="0.35">
+      <c r="A31" s="14"/>
+      <c r="B31" s="14"/>
+      <c r="C31" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="48.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A32" s="14"/>
+      <c r="B32" s="18"/>
+      <c r="C32" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="36.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A33" s="14"/>
+      <c r="B33" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C33" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="D33" s="20"/>
+    </row>
+    <row r="34" spans="1:4" ht="24.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A34" s="16"/>
+      <c r="B34" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C34" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="D34" s="22"/>
+    </row>
+    <row r="35" spans="1:4" ht="85" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A35" s="39" t="s">
+        <v>63</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="48" x14ac:dyDescent="0.35">
+      <c r="A36" s="14"/>
+      <c r="B36" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D36" s="44" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="48" x14ac:dyDescent="0.35">
+      <c r="A37" s="14"/>
+      <c r="B37" s="14"/>
+      <c r="C37" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D37" s="45"/>
+    </row>
+    <row r="38" spans="1:4" ht="60.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A38" s="14"/>
+      <c r="B38" s="18"/>
+      <c r="C38" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D38" s="46"/>
+    </row>
+    <row r="39" spans="1:4" ht="48" x14ac:dyDescent="0.35">
+      <c r="A39" s="14"/>
+      <c r="B39" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="48" x14ac:dyDescent="0.35">
+      <c r="A40" s="14"/>
+      <c r="B40" s="14"/>
+      <c r="C40" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="60.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A41" s="16"/>
+      <c r="B41" s="16"/>
+      <c r="C41" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A42" s="39" t="s">
+        <v>67</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C42" s="40" t="s">
+        <v>44</v>
+      </c>
+      <c r="D42" s="41"/>
+    </row>
+    <row r="43" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A43" s="14"/>
+      <c r="B43" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C43" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="D43" s="43"/>
+    </row>
+    <row r="44" spans="1:4" ht="24.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A44" s="14"/>
+      <c r="B44" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C44" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="D44" s="20"/>
+    </row>
+    <row r="45" spans="1:4" ht="48" x14ac:dyDescent="0.35">
+      <c r="A45" s="14"/>
+      <c r="B45" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="36" x14ac:dyDescent="0.35">
+      <c r="A46" s="14"/>
+      <c r="B46" s="14"/>
+      <c r="C46" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D46" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="24" x14ac:dyDescent="0.35">
+      <c r="A47" s="14"/>
+      <c r="B47" s="14"/>
+      <c r="C47" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D47" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="48" x14ac:dyDescent="0.35">
+      <c r="A48" s="14"/>
+      <c r="B48" s="14"/>
+      <c r="C48" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="36" x14ac:dyDescent="0.35">
+      <c r="A49" s="14"/>
+      <c r="B49" s="14"/>
+      <c r="C49" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D49" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="24" x14ac:dyDescent="0.35">
+      <c r="A50" s="14"/>
+      <c r="B50" s="14"/>
+      <c r="C50" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D50" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="48" x14ac:dyDescent="0.35">
+      <c r="A51" s="14"/>
+      <c r="B51" s="14"/>
+      <c r="C51" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="48.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A52" s="14"/>
+      <c r="B52" s="18"/>
+      <c r="C52" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D52" s="8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="36.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A53" s="14"/>
+      <c r="B53" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C53" s="47" t="s">
+        <v>60</v>
+      </c>
+      <c r="D53" s="48"/>
+    </row>
+    <row r="54" spans="1:4" ht="24.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A54" s="16"/>
+      <c r="B54" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C54" s="49" t="s">
+        <v>62</v>
+      </c>
+      <c r="D54" s="50"/>
+    </row>
+    <row r="55" spans="1:4" ht="108" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A55" s="39" t="s">
+        <v>68</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C55" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="D55" s="13"/>
+    </row>
+    <row r="56" spans="1:4" ht="120" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A56" s="16"/>
+      <c r="B56" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C56" s="49" t="s">
+        <v>72</v>
+      </c>
+      <c r="D56" s="50"/>
+    </row>
+    <row r="57" spans="1:4" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A57" s="39" t="s">
+        <v>73</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C57" s="40" t="s">
+        <v>75</v>
+      </c>
+      <c r="D57" s="41"/>
+    </row>
+    <row r="58" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A58" s="14"/>
+      <c r="B58" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C58" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="D58" s="20"/>
+    </row>
+    <row r="59" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A59" s="14"/>
+      <c r="B59" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C59" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="D59" s="20"/>
+    </row>
+    <row r="60" spans="1:4" ht="24.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A60" s="14"/>
+      <c r="B60" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C60" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="D60" s="20"/>
+    </row>
+    <row r="61" spans="1:4" ht="24.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A61" s="14"/>
+      <c r="B61" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C61" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="D61" s="20"/>
+    </row>
+    <row r="62" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A62" s="14"/>
+      <c r="B62" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="C62" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="D62" s="20"/>
+    </row>
+    <row r="63" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A63" s="14"/>
+      <c r="B63" s="18"/>
+      <c r="C63" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="D63" s="20"/>
+    </row>
+    <row r="64" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A64" s="16"/>
+      <c r="B64" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C64" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="D64" s="22"/>
+    </row>
+    <row r="65" spans="1:4" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A65" s="39" t="s">
+        <v>89</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C65" s="40" t="s">
+        <v>91</v>
+      </c>
+      <c r="D65" s="41"/>
+    </row>
+    <row r="66" spans="1:4" ht="36.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A66" s="14"/>
+      <c r="B66" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C66" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="D66" s="20"/>
+    </row>
+    <row r="67" spans="1:4" ht="36.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A67" s="14"/>
+      <c r="B67" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C67" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="D67" s="20"/>
+    </row>
+    <row r="68" spans="1:4" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A68" s="16"/>
+      <c r="B68" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="C68" s="51" t="s">
+        <v>97</v>
+      </c>
+      <c r="D68" s="52"/>
+    </row>
+    <row r="69" spans="1:4" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A69" s="39" t="s">
+        <v>98</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C69" s="40" t="s">
+        <v>100</v>
+      </c>
+      <c r="D69" s="41"/>
+    </row>
+    <row r="70" spans="1:4" ht="24.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A70" s="14"/>
+      <c r="B70" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C70" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="D70" s="20"/>
+    </row>
+    <row r="71" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A71" s="14"/>
+      <c r="B71" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C71" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="D71" s="20"/>
+    </row>
+    <row r="72" spans="1:4" ht="24.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A72" s="14"/>
+      <c r="B72" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C72" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="D72" s="20"/>
+    </row>
+    <row r="73" spans="1:4" ht="24.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A73" s="14"/>
+      <c r="B73" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C73" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="D73" s="20"/>
+    </row>
+    <row r="74" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A74" s="16"/>
+      <c r="B74" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="C74" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="D74" s="22"/>
+    </row>
+    <row r="75" spans="1:4" ht="24" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A75" s="39" t="s">
+        <v>110</v>
+      </c>
+      <c r="B75" s="39" t="s">
+        <v>111</v>
+      </c>
+      <c r="C75" s="53" t="s">
+        <v>112</v>
+      </c>
+      <c r="D75" s="54"/>
+    </row>
+    <row r="76" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A76" s="14"/>
+      <c r="B76" s="18"/>
+      <c r="C76" s="55" t="s">
+        <v>113</v>
+      </c>
+      <c r="D76" s="56"/>
+    </row>
+    <row r="77" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A77" s="16"/>
+      <c r="B77" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="C77" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="D77" s="22"/>
+    </row>
+    <row r="78" spans="1:4" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A78" s="39" t="s">
+        <v>116</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C78" s="40" t="s">
+        <v>118</v>
+      </c>
+      <c r="D78" s="41"/>
+    </row>
+    <row r="79" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A79" s="14"/>
+      <c r="B79" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="C79" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="D79" s="20"/>
+    </row>
+    <row r="80" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A80" s="14"/>
+      <c r="B80" s="18"/>
+      <c r="C80" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="D80" s="20"/>
+    </row>
+    <row r="81" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A81" s="14"/>
+      <c r="B81" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="C81" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="D81" s="20"/>
+    </row>
+    <row r="82" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A82" s="16"/>
+      <c r="B82" s="16"/>
+      <c r="C82" s="21" t="s">
+        <v>124</v>
+      </c>
+      <c r="D82" s="22"/>
+    </row>
+    <row r="83" spans="1:4" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A83" s="39" t="s">
+        <v>125</v>
+      </c>
+      <c r="B83" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C83" s="40" t="s">
+        <v>127</v>
+      </c>
+      <c r="D83" s="41"/>
+    </row>
+    <row r="84" spans="1:4" ht="36.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A84" s="16"/>
+      <c r="B84" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="C84" s="21" t="s">
+        <v>129</v>
+      </c>
+      <c r="D84" s="22"/>
+    </row>
+    <row r="85" spans="1:4" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A85" s="29" t="s">
+        <v>130</v>
+      </c>
+      <c r="B85" s="30"/>
+      <c r="C85" s="40" t="s">
+        <v>131</v>
+      </c>
+      <c r="D85" s="41"/>
+    </row>
+    <row r="86" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A86" s="28"/>
+      <c r="B86" s="17"/>
+      <c r="C86" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="D86" s="20"/>
+    </row>
+    <row r="87" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A87" s="23"/>
+      <c r="B87" s="57"/>
+      <c r="C87" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="D87" s="22"/>
+    </row>
+    <row r="88" spans="1:4" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A88" s="29" t="s">
+        <v>134</v>
+      </c>
+      <c r="B88" s="30"/>
+      <c r="C88" s="40" t="s">
         <v>135</v>
       </c>
-      <c r="B12" s="11"/>
-      <c r="C12" s="52" t="s">
+      <c r="D88" s="41"/>
+    </row>
+    <row r="89" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A89" s="28"/>
+      <c r="B89" s="17"/>
+      <c r="C89" s="19" t="s">
         <v>136</v>
       </c>
-      <c r="D12" s="53"/>
-    </row>
-    <row r="13" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="12"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="54"/>
-      <c r="D13" s="55"/>
-    </row>
-    <row r="14" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="50"/>
-      <c r="B14" s="51"/>
-      <c r="C14" s="56"/>
-      <c r="D14" s="57"/>
-    </row>
-    <row r="15" spans="1:4" ht="24.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="24" x14ac:dyDescent="0.35">
-      <c r="A16" s="25"/>
-      <c r="B16" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A17" s="25"/>
-      <c r="B17" s="25"/>
-      <c r="C17" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="24.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="25"/>
-      <c r="B18" s="26"/>
-      <c r="C18" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A19" s="25"/>
-      <c r="B19" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A20" s="25"/>
-      <c r="B20" s="25"/>
-      <c r="C20" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="23"/>
-      <c r="B21" s="23"/>
-      <c r="C21" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C22" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="D22" s="17"/>
-    </row>
-    <row r="23" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="25"/>
-      <c r="B23" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C23" s="40" t="s">
-        <v>41</v>
-      </c>
-      <c r="D23" s="41"/>
-    </row>
-    <row r="24" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="25"/>
-      <c r="B24" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C24" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="D24" s="19"/>
-    </row>
-    <row r="25" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="25"/>
-      <c r="B25" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="C25" s="58" t="s">
+      <c r="D89" s="20"/>
+    </row>
+    <row r="90" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A90" s="28"/>
+      <c r="B90" s="17"/>
+      <c r="C90" s="19" t="s">
         <v>137</v>
       </c>
-      <c r="D25" s="5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A26" s="25"/>
-      <c r="B26" s="25"/>
-      <c r="C26" s="38"/>
-      <c r="D26" s="7" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A27" s="25"/>
-      <c r="B27" s="25"/>
-      <c r="C27" s="38"/>
-      <c r="D27" s="7" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="24" x14ac:dyDescent="0.35">
-      <c r="A28" s="25"/>
-      <c r="B28" s="25"/>
-      <c r="C28" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A29" s="25"/>
-      <c r="B29" s="25"/>
-      <c r="C29" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="D29" s="7" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A30" s="25"/>
-      <c r="B30" s="25"/>
-      <c r="C30" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="D30" s="7" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="24" x14ac:dyDescent="0.35">
-      <c r="A31" s="25"/>
-      <c r="B31" s="25"/>
-      <c r="C31" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="24.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="25"/>
-      <c r="B32" s="26"/>
-      <c r="C32" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="D32" s="8" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="24.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A33" s="25"/>
-      <c r="B33" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C33" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="D33" s="19"/>
-    </row>
-    <row r="34" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="23"/>
-      <c r="B34" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="C34" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="D34" s="21"/>
-    </row>
-    <row r="35" spans="1:4" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="24" x14ac:dyDescent="0.35">
-      <c r="A36" s="25"/>
-      <c r="B36" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D36" s="37" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A37" s="25"/>
-      <c r="B37" s="25"/>
-      <c r="C37" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D37" s="38"/>
-    </row>
-    <row r="38" spans="1:4" ht="24.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A38" s="25"/>
-      <c r="B38" s="26"/>
-      <c r="C38" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D38" s="39"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A39" s="25"/>
-      <c r="B39" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D39" s="5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A40" s="25"/>
-      <c r="B40" s="25"/>
-      <c r="C40" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A41" s="23"/>
-      <c r="B41" s="23"/>
-      <c r="C41" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D41" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A42" s="24" t="s">
-        <v>62</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C42" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="D42" s="17"/>
-    </row>
-    <row r="43" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A43" s="25"/>
-      <c r="B43" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C43" s="40" t="s">
-        <v>41</v>
-      </c>
-      <c r="D43" s="41"/>
-    </row>
-    <row r="44" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A44" s="25"/>
-      <c r="B44" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C44" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="D44" s="19"/>
-    </row>
-    <row r="45" spans="1:4" ht="24" x14ac:dyDescent="0.35">
-      <c r="A45" s="25"/>
-      <c r="B45" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="C45" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="D45" s="5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A46" s="25"/>
-      <c r="B46" s="25"/>
-      <c r="C46" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="D46" s="7" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A47" s="25"/>
-      <c r="B47" s="25"/>
-      <c r="C47" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="D47" s="7" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="24" x14ac:dyDescent="0.35">
-      <c r="A48" s="25"/>
-      <c r="B48" s="25"/>
-      <c r="C48" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D48" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A49" s="25"/>
-      <c r="B49" s="25"/>
-      <c r="C49" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="D49" s="7" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A50" s="25"/>
-      <c r="B50" s="25"/>
-      <c r="C50" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="D50" s="7" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" ht="24" x14ac:dyDescent="0.35">
-      <c r="A51" s="25"/>
-      <c r="B51" s="25"/>
-      <c r="C51" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D51" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" ht="24.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A52" s="25"/>
-      <c r="B52" s="26"/>
-      <c r="C52" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="D52" s="8" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" ht="24.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A53" s="25"/>
-      <c r="B53" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C53" s="42" t="s">
-        <v>55</v>
-      </c>
-      <c r="D53" s="43"/>
-    </row>
-    <row r="54" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A54" s="23"/>
-      <c r="B54" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="C54" s="33" t="s">
-        <v>57</v>
-      </c>
-      <c r="D54" s="34"/>
-    </row>
-    <row r="55" spans="1:4" ht="108" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A55" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C55" s="35" t="s">
-        <v>65</v>
-      </c>
-      <c r="D55" s="36"/>
-    </row>
-    <row r="56" spans="1:4" ht="120" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A56" s="23"/>
-      <c r="B56" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="C56" s="33" t="s">
-        <v>67</v>
-      </c>
-      <c r="D56" s="34"/>
-    </row>
-    <row r="57" spans="1:4" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A57" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C57" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="D57" s="17"/>
-    </row>
-    <row r="58" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A58" s="25"/>
-      <c r="B58" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="C58" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="D58" s="19"/>
-    </row>
-    <row r="59" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A59" s="25"/>
-      <c r="B59" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C59" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="D59" s="19"/>
-    </row>
-    <row r="60" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A60" s="25"/>
-      <c r="B60" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C60" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="D60" s="19"/>
-    </row>
-    <row r="61" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A61" s="25"/>
-      <c r="B61" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C61" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="D61" s="19"/>
-    </row>
-    <row r="62" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A62" s="25"/>
-      <c r="B62" s="22" t="s">
-        <v>79</v>
-      </c>
-      <c r="C62" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="D62" s="19"/>
-    </row>
-    <row r="63" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A63" s="25"/>
-      <c r="B63" s="26"/>
-      <c r="C63" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="D63" s="19"/>
-    </row>
-    <row r="64" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A64" s="23"/>
-      <c r="B64" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="C64" s="20" t="s">
-        <v>83</v>
-      </c>
-      <c r="D64" s="21"/>
-    </row>
-    <row r="65" spans="1:4" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A65" s="24" t="s">
-        <v>84</v>
-      </c>
-      <c r="B65" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C65" s="16" t="s">
-        <v>86</v>
-      </c>
-      <c r="D65" s="17"/>
-    </row>
-    <row r="66" spans="1:4" ht="24.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A66" s="25"/>
-      <c r="B66" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="C66" s="18" t="s">
-        <v>88</v>
-      </c>
-      <c r="D66" s="19"/>
-    </row>
-    <row r="67" spans="1:4" ht="24.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A67" s="25"/>
-      <c r="B67" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="C67" s="18" t="s">
-        <v>90</v>
-      </c>
-      <c r="D67" s="19"/>
-    </row>
-    <row r="68" spans="1:4" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A68" s="23"/>
-      <c r="B68" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="C68" s="31" t="s">
-        <v>92</v>
-      </c>
-      <c r="D68" s="32"/>
-    </row>
-    <row r="69" spans="1:4" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A69" s="24" t="s">
-        <v>93</v>
-      </c>
-      <c r="B69" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="C69" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="D69" s="17"/>
-    </row>
-    <row r="70" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A70" s="25"/>
-      <c r="B70" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="C70" s="18" t="s">
-        <v>97</v>
-      </c>
-      <c r="D70" s="19"/>
-    </row>
-    <row r="71" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A71" s="25"/>
-      <c r="B71" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="C71" s="18" t="s">
-        <v>98</v>
-      </c>
-      <c r="D71" s="19"/>
-    </row>
-    <row r="72" spans="1:4" ht="24.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A72" s="25"/>
-      <c r="B72" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="C72" s="18" t="s">
-        <v>100</v>
-      </c>
-      <c r="D72" s="19"/>
-    </row>
-    <row r="73" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A73" s="25"/>
-      <c r="B73" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="C73" s="18" t="s">
-        <v>102</v>
-      </c>
-      <c r="D73" s="19"/>
-    </row>
-    <row r="74" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A74" s="23"/>
-      <c r="B74" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="C74" s="20" t="s">
-        <v>104</v>
-      </c>
-      <c r="D74" s="21"/>
-    </row>
-    <row r="75" spans="1:4" ht="24" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A75" s="24" t="s">
-        <v>105</v>
-      </c>
-      <c r="B75" s="24" t="s">
-        <v>106</v>
-      </c>
-      <c r="C75" s="27" t="s">
-        <v>107</v>
-      </c>
-      <c r="D75" s="28"/>
-    </row>
-    <row r="76" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A76" s="25"/>
-      <c r="B76" s="26"/>
-      <c r="C76" s="29" t="s">
-        <v>108</v>
-      </c>
-      <c r="D76" s="30"/>
-    </row>
-    <row r="77" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A77" s="23"/>
-      <c r="B77" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="C77" s="20" t="s">
-        <v>110</v>
-      </c>
-      <c r="D77" s="21"/>
-    </row>
-    <row r="78" spans="1:4" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A78" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="B78" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="C78" s="16" t="s">
-        <v>113</v>
-      </c>
-      <c r="D78" s="17"/>
-    </row>
-    <row r="79" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A79" s="25"/>
-      <c r="B79" s="22" t="s">
-        <v>114</v>
-      </c>
-      <c r="C79" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="D79" s="19"/>
-    </row>
-    <row r="80" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A80" s="25"/>
-      <c r="B80" s="26"/>
-      <c r="C80" s="18" t="s">
-        <v>116</v>
-      </c>
-      <c r="D80" s="19"/>
-    </row>
-    <row r="81" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A81" s="25"/>
-      <c r="B81" s="22" t="s">
-        <v>117</v>
-      </c>
-      <c r="C81" s="18" t="s">
-        <v>118</v>
-      </c>
-      <c r="D81" s="19"/>
-    </row>
-    <row r="82" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A82" s="23"/>
-      <c r="B82" s="23"/>
-      <c r="C82" s="20" t="s">
-        <v>119</v>
-      </c>
-      <c r="D82" s="21"/>
-    </row>
-    <row r="83" spans="1:4" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A83" s="24" t="s">
-        <v>120</v>
-      </c>
-      <c r="B83" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="C83" s="16" t="s">
-        <v>122</v>
-      </c>
-      <c r="D83" s="17"/>
-    </row>
-    <row r="84" spans="1:4" ht="24.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A84" s="23"/>
-      <c r="B84" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="C84" s="20" t="s">
-        <v>124</v>
-      </c>
-      <c r="D84" s="21"/>
-    </row>
-    <row r="85" spans="1:4" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A85" s="10" t="s">
-        <v>125</v>
-      </c>
-      <c r="B85" s="11"/>
-      <c r="C85" s="16" t="s">
-        <v>126</v>
-      </c>
-      <c r="D85" s="17"/>
-    </row>
-    <row r="86" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A86" s="12"/>
-      <c r="B86" s="13"/>
-      <c r="C86" s="18" t="s">
-        <v>127</v>
-      </c>
-      <c r="D86" s="19"/>
-    </row>
-    <row r="87" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A87" s="14"/>
-      <c r="B87" s="15"/>
-      <c r="C87" s="20" t="s">
-        <v>128</v>
-      </c>
-      <c r="D87" s="21"/>
-    </row>
-    <row r="88" spans="1:4" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A88" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="B88" s="11"/>
-      <c r="C88" s="16" t="s">
-        <v>130</v>
-      </c>
-      <c r="D88" s="17"/>
-    </row>
-    <row r="89" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A89" s="12"/>
-      <c r="B89" s="13"/>
-      <c r="C89" s="18" t="s">
-        <v>131</v>
-      </c>
-      <c r="D89" s="19"/>
-    </row>
-    <row r="90" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A90" s="12"/>
-      <c r="B90" s="13"/>
-      <c r="C90" s="18" t="s">
-        <v>132</v>
-      </c>
-      <c r="D90" s="19"/>
+      <c r="D90" s="20"/>
     </row>
     <row r="91" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A91" s="12"/>
-      <c r="B91" s="13"/>
-      <c r="C91" s="18" t="s">
-        <v>133</v>
-      </c>
-      <c r="D91" s="19"/>
+      <c r="A91" s="28"/>
+      <c r="B91" s="17"/>
+      <c r="C91" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="D91" s="20"/>
     </row>
     <row r="92" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A92" s="14"/>
-      <c r="B92" s="15"/>
-      <c r="C92" s="20" t="s">
-        <v>134</v>
-      </c>
-      <c r="D92" s="21"/>
+      <c r="A92" s="23"/>
+      <c r="B92" s="57"/>
+      <c r="C92" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="D92" s="22"/>
     </row>
     <row r="93" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
-  <mergeCells count="91">
+  <mergeCells count="94">
+    <mergeCell ref="A85:B87"/>
+    <mergeCell ref="C85:D85"/>
+    <mergeCell ref="C86:D86"/>
+    <mergeCell ref="C87:D87"/>
+    <mergeCell ref="A88:B92"/>
+    <mergeCell ref="C88:D88"/>
+    <mergeCell ref="C89:D89"/>
+    <mergeCell ref="C90:D90"/>
+    <mergeCell ref="C91:D91"/>
+    <mergeCell ref="C92:D92"/>
+    <mergeCell ref="B81:B82"/>
+    <mergeCell ref="C81:D81"/>
+    <mergeCell ref="C82:D82"/>
+    <mergeCell ref="A83:A84"/>
+    <mergeCell ref="C83:D83"/>
+    <mergeCell ref="C84:D84"/>
+    <mergeCell ref="A75:A77"/>
+    <mergeCell ref="B75:B76"/>
+    <mergeCell ref="C75:D75"/>
+    <mergeCell ref="C76:D76"/>
+    <mergeCell ref="C77:D77"/>
+    <mergeCell ref="A78:A82"/>
+    <mergeCell ref="C78:D78"/>
+    <mergeCell ref="B79:B80"/>
+    <mergeCell ref="C79:D79"/>
+    <mergeCell ref="C80:D80"/>
+    <mergeCell ref="A69:A74"/>
+    <mergeCell ref="C69:D69"/>
+    <mergeCell ref="C70:D70"/>
+    <mergeCell ref="C71:D71"/>
+    <mergeCell ref="C72:D72"/>
+    <mergeCell ref="C73:D73"/>
+    <mergeCell ref="C74:D74"/>
+    <mergeCell ref="B62:B63"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="C63:D63"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="A65:A68"/>
+    <mergeCell ref="C65:D65"/>
+    <mergeCell ref="C66:D66"/>
+    <mergeCell ref="C67:D67"/>
+    <mergeCell ref="C68:D68"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="A55:A56"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="C56:D56"/>
+    <mergeCell ref="A57:A64"/>
+    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="C58:D58"/>
+    <mergeCell ref="C59:D59"/>
+    <mergeCell ref="C60:D60"/>
+    <mergeCell ref="C61:D61"/>
+    <mergeCell ref="A35:A41"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="D36:D38"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="A42:A54"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="B45:B52"/>
+    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="A15:A21"/>
+    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="A22:A34"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="B25:B32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:D11"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:A9"/>
@@ -2915,87 +3045,6 @@
     <mergeCell ref="B6:B9"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="A12:B14"/>
-    <mergeCell ref="C12:D14"/>
-    <mergeCell ref="A15:A21"/>
-    <mergeCell ref="B16:B18"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="A22:A34"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="B25:B32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C25:C27"/>
-    <mergeCell ref="A35:A41"/>
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="D36:D38"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="A42:A54"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="B45:B52"/>
-    <mergeCell ref="C53:D53"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="A55:A56"/>
-    <mergeCell ref="C55:D55"/>
-    <mergeCell ref="C56:D56"/>
-    <mergeCell ref="A57:A64"/>
-    <mergeCell ref="C57:D57"/>
-    <mergeCell ref="C58:D58"/>
-    <mergeCell ref="C59:D59"/>
-    <mergeCell ref="C60:D60"/>
-    <mergeCell ref="C61:D61"/>
-    <mergeCell ref="B62:B63"/>
-    <mergeCell ref="C62:D62"/>
-    <mergeCell ref="C63:D63"/>
-    <mergeCell ref="C64:D64"/>
-    <mergeCell ref="A65:A68"/>
-    <mergeCell ref="C65:D65"/>
-    <mergeCell ref="C66:D66"/>
-    <mergeCell ref="C67:D67"/>
-    <mergeCell ref="C68:D68"/>
-    <mergeCell ref="A69:A74"/>
-    <mergeCell ref="C69:D69"/>
-    <mergeCell ref="C70:D70"/>
-    <mergeCell ref="C71:D71"/>
-    <mergeCell ref="C72:D72"/>
-    <mergeCell ref="C73:D73"/>
-    <mergeCell ref="C74:D74"/>
-    <mergeCell ref="A75:A77"/>
-    <mergeCell ref="B75:B76"/>
-    <mergeCell ref="C75:D75"/>
-    <mergeCell ref="C76:D76"/>
-    <mergeCell ref="C77:D77"/>
-    <mergeCell ref="B81:B82"/>
-    <mergeCell ref="C81:D81"/>
-    <mergeCell ref="C82:D82"/>
-    <mergeCell ref="A83:A84"/>
-    <mergeCell ref="C83:D83"/>
-    <mergeCell ref="C84:D84"/>
-    <mergeCell ref="A78:A82"/>
-    <mergeCell ref="C78:D78"/>
-    <mergeCell ref="B79:B80"/>
-    <mergeCell ref="C79:D79"/>
-    <mergeCell ref="C80:D80"/>
-    <mergeCell ref="A85:B87"/>
-    <mergeCell ref="C85:D85"/>
-    <mergeCell ref="C86:D86"/>
-    <mergeCell ref="C87:D87"/>
-    <mergeCell ref="A88:B92"/>
-    <mergeCell ref="C88:D88"/>
-    <mergeCell ref="C89:D89"/>
-    <mergeCell ref="C90:D90"/>
-    <mergeCell ref="C91:D91"/>
-    <mergeCell ref="C92:D92"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
trying borders per page and new underline pre-placed in Excel
</commit_message>
<xml_diff>
--- a/src/docs/SampleTable.xlsx
+++ b/src/docs/SampleTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dctlchn\src\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CABC6C6A-76AE-4104-8D3C-B75D12072FFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0294DFD2-9331-4712-B44C-F52D032D763B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{52CCC0D4-432A-4BEC-84E5-9AE94DB33649}"/>
   </bookViews>
@@ -989,12 +989,6 @@
     <t>External Illuminator (IZS Series)</t>
   </si>
   <si>
-    <t>IZA800[.underline]#G#</t>
-  </si>
-  <si>
-    <t>IZA800[.underline]#GW#</t>
-  </si>
-  <si>
     <t>LPR Capture Distance* (for U.S.A. plates)</t>
   </si>
   <si>
@@ -1137,6 +1131,12 @@
   </si>
   <si>
     <t>(W x H x D) 6.7” x 4.7” x 17.7” (171 mm x 119 mm x 451 mm)</t>
+  </si>
+  <si>
+    <t>IZA800+++&lt;u&gt;G&lt;/u&gt;+++</t>
+  </si>
+  <si>
+    <t>IZA800+++&lt;u&gt;GW&lt;/u&gt;+++</t>
   </si>
 </sst>
 </file>
@@ -1496,136 +1496,136 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1945,7 +1945,7 @@
   <dimension ref="A1:D82"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13:D13"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1956,23 +1956,23 @@
     <col min="4" max="4" width="24.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:4" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
+      <c r="B1" s="51"/>
       <c r="C1" s="1" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="11"/>
+      <c r="B2" s="20"/>
       <c r="C2" s="4" t="s">
         <v>2</v>
       </c>
@@ -1981,115 +1981,115 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="17"/>
+      <c r="D3" s="14"/>
     </row>
     <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="13"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="16" t="s">
+      <c r="A4" s="9"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="17"/>
+      <c r="D4" s="14"/>
     </row>
     <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="13"/>
-      <c r="B5" s="15"/>
-      <c r="C5" s="16" t="s">
+      <c r="A5" s="9"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="17"/>
+      <c r="D5" s="14"/>
     </row>
     <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="13"/>
-      <c r="B6" s="12" t="s">
+      <c r="A6" s="9"/>
+      <c r="B6" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="17"/>
+      <c r="D6" s="14"/>
     </row>
     <row r="7" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="13"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="16" t="s">
+      <c r="A7" s="9"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="17"/>
+      <c r="D7" s="14"/>
     </row>
     <row r="8" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="13"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="16" t="s">
+      <c r="A8" s="9"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="17"/>
+      <c r="D8" s="14"/>
     </row>
     <row r="9" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="14"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="18" t="s">
+      <c r="A9" s="10"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="19"/>
+      <c r="D9" s="24"/>
     </row>
     <row r="10" spans="1:4" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="21"/>
-      <c r="C10" s="22" t="s">
+      <c r="B10" s="45"/>
+      <c r="C10" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="23"/>
+      <c r="D10" s="47"/>
     </row>
     <row r="11" spans="1:4" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="20" t="s">
+      <c r="A11" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="21"/>
-      <c r="C11" s="22" t="s">
+      <c r="B11" s="45"/>
+      <c r="C11" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="23"/>
+      <c r="D11" s="47"/>
     </row>
     <row r="12" spans="1:4" ht="24" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="30" t="s">
-        <v>127</v>
-      </c>
-      <c r="B12" s="31"/>
-      <c r="C12" s="24" t="s">
+      <c r="A12" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="B12" s="26"/>
+      <c r="C12" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="25"/>
+      <c r="D12" s="49"/>
     </row>
     <row r="13" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="32"/>
-      <c r="B13" s="33"/>
-      <c r="C13" s="26" t="s">
+      <c r="A13" s="27"/>
+      <c r="B13" s="28"/>
+      <c r="C13" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="27"/>
+      <c r="D13" s="39"/>
     </row>
     <row r="14" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="34"/>
-      <c r="B14" s="35"/>
-      <c r="C14" s="28" t="s">
+      <c r="A14" s="42"/>
+      <c r="B14" s="43"/>
+      <c r="C14" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="29"/>
-    </row>
-    <row r="15" spans="1:4" ht="84.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="12" t="s">
+      <c r="D14" s="41"/>
+    </row>
+    <row r="15" spans="1:4" ht="24.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="15" t="s">
         <v>20</v>
       </c>
       <c r="B15" s="7" t="s">
@@ -2102,9 +2102,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="48" x14ac:dyDescent="0.35">
-      <c r="A16" s="13"/>
-      <c r="B16" s="12" t="s">
+    <row r="16" spans="1:4" ht="24" x14ac:dyDescent="0.35">
+      <c r="A16" s="9"/>
+      <c r="B16" s="15" t="s">
         <v>24</v>
       </c>
       <c r="C16" s="5" t="s">
@@ -2114,9 +2114,9 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="48" x14ac:dyDescent="0.35">
-      <c r="A17" s="13"/>
-      <c r="B17" s="13"/>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" s="9"/>
+      <c r="B17" s="9"/>
       <c r="C17" s="5" t="s">
         <v>26</v>
       </c>
@@ -2124,9 +2124,9 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="60.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="13"/>
-      <c r="B18" s="15"/>
+    <row r="18" spans="1:4" ht="24.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="9"/>
+      <c r="B18" s="16"/>
       <c r="C18" s="6" t="s">
         <v>27</v>
       </c>
@@ -2134,9 +2134,9 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="48" x14ac:dyDescent="0.35">
-      <c r="A19" s="13"/>
-      <c r="B19" s="12" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" s="9"/>
+      <c r="B19" s="15" t="s">
         <v>31</v>
       </c>
       <c r="C19" s="5" t="s">
@@ -2146,9 +2146,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="48" x14ac:dyDescent="0.35">
-      <c r="A20" s="13"/>
-      <c r="B20" s="13"/>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" s="9"/>
+      <c r="B20" s="9"/>
       <c r="C20" s="5" t="s">
         <v>33</v>
       </c>
@@ -2156,9 +2156,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="60.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="14"/>
-      <c r="B21" s="14"/>
+    <row r="21" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="10"/>
+      <c r="B21" s="10"/>
       <c r="C21" s="2" t="s">
         <v>34</v>
       </c>
@@ -2166,92 +2166,92 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="36" t="s">
+    <row r="22" spans="1:4" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="8" t="s">
         <v>38</v>
       </c>
       <c r="B22" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C22" s="37" t="s">
+      <c r="C22" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="D22" s="38"/>
+      <c r="D22" s="12"/>
     </row>
     <row r="23" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="13"/>
+      <c r="A23" s="9"/>
       <c r="B23" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C23" s="39" t="s">
+      <c r="C23" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="D23" s="40"/>
-    </row>
-    <row r="24" spans="1:4" ht="24.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="13"/>
+      <c r="D23" s="18"/>
+    </row>
+    <row r="24" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="9"/>
       <c r="B24" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="C24" s="16" t="s">
+      <c r="C24" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="D24" s="17"/>
-    </row>
-    <row r="25" spans="1:4" ht="120" x14ac:dyDescent="0.35">
-      <c r="A25" s="13"/>
-      <c r="B25" s="12" t="s">
+      <c r="D24" s="14"/>
+    </row>
+    <row r="25" spans="1:4" ht="36" x14ac:dyDescent="0.35">
+      <c r="A25" s="9"/>
+      <c r="B25" s="15" t="s">
         <v>45</v>
       </c>
       <c r="C25" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="36" x14ac:dyDescent="0.35">
+      <c r="A26" s="9"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="36.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A27" s="9"/>
+      <c r="B27" s="16"/>
+      <c r="C27" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="D27" s="6" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="120" x14ac:dyDescent="0.35">
-      <c r="A26" s="13"/>
-      <c r="B26" s="13"/>
-      <c r="C26" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="96.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="13"/>
-      <c r="B27" s="15"/>
-      <c r="C27" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="36.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="13"/>
+    <row r="28" spans="1:4" ht="24.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A28" s="9"/>
       <c r="B28" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C28" s="16" t="s">
+      <c r="C28" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="D28" s="17"/>
-    </row>
-    <row r="29" spans="1:4" ht="24.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="14"/>
+      <c r="D28" s="14"/>
+    </row>
+    <row r="29" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A29" s="10"/>
       <c r="B29" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C29" s="18" t="s">
+      <c r="C29" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="D29" s="19"/>
-    </row>
-    <row r="30" spans="1:4" ht="85" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="36" t="s">
+      <c r="D29" s="24"/>
+    </row>
+    <row r="30" spans="1:4" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A30" s="8" t="s">
         <v>50</v>
       </c>
       <c r="B30" s="7" t="s">
@@ -2264,37 +2264,37 @@
         <v>52</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="48" x14ac:dyDescent="0.35">
-      <c r="A31" s="13"/>
-      <c r="B31" s="12" t="s">
+    <row r="31" spans="1:4" ht="24" x14ac:dyDescent="0.35">
+      <c r="A31" s="9"/>
+      <c r="B31" s="15" t="s">
         <v>24</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D31" s="41" t="s">
+      <c r="D31" s="35" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="48" x14ac:dyDescent="0.35">
-      <c r="A32" s="13"/>
-      <c r="B32" s="13"/>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A32" s="9"/>
+      <c r="B32" s="9"/>
       <c r="C32" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D32" s="42"/>
-    </row>
-    <row r="33" spans="1:4" ht="60.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A33" s="13"/>
-      <c r="B33" s="15"/>
+      <c r="D32" s="36"/>
+    </row>
+    <row r="33" spans="1:4" ht="24.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A33" s="9"/>
+      <c r="B33" s="16"/>
       <c r="C33" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D33" s="43"/>
-    </row>
-    <row r="34" spans="1:4" ht="48" x14ac:dyDescent="0.35">
-      <c r="A34" s="13"/>
-      <c r="B34" s="12" t="s">
+      <c r="D33" s="37"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A34" s="9"/>
+      <c r="B34" s="15" t="s">
         <v>31</v>
       </c>
       <c r="C34" s="5" t="s">
@@ -2304,9 +2304,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="48" x14ac:dyDescent="0.35">
-      <c r="A35" s="13"/>
-      <c r="B35" s="13"/>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A35" s="9"/>
+      <c r="B35" s="9"/>
       <c r="C35" s="5" t="s">
         <v>33</v>
       </c>
@@ -2314,9 +2314,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="60.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="14"/>
-      <c r="B36" s="14"/>
+    <row r="36" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A36" s="10"/>
+      <c r="B36" s="10"/>
       <c r="C36" s="2" t="s">
         <v>34</v>
       </c>
@@ -2324,479 +2324,515 @@
         <v>37</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A37" s="36" t="s">
+    <row r="37" spans="1:4" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A37" s="8" t="s">
         <v>54</v>
       </c>
       <c r="B37" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C37" s="37" t="s">
+      <c r="C37" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="D37" s="38"/>
+      <c r="D37" s="12"/>
     </row>
     <row r="38" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A38" s="13"/>
+      <c r="A38" s="9"/>
       <c r="B38" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C38" s="39" t="s">
+      <c r="C38" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="D38" s="40"/>
-    </row>
-    <row r="39" spans="1:4" ht="24.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A39" s="13"/>
+      <c r="D38" s="18"/>
+    </row>
+    <row r="39" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A39" s="9"/>
       <c r="B39" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="C39" s="16" t="s">
+      <c r="C39" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="D39" s="17"/>
-    </row>
-    <row r="40" spans="1:4" ht="120" x14ac:dyDescent="0.35">
-      <c r="A40" s="13"/>
-      <c r="B40" s="12" t="s">
+      <c r="D39" s="14"/>
+    </row>
+    <row r="40" spans="1:4" ht="36" x14ac:dyDescent="0.35">
+      <c r="A40" s="9"/>
+      <c r="B40" s="15" t="s">
         <v>45</v>
       </c>
       <c r="C40" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="36" x14ac:dyDescent="0.35">
+      <c r="A41" s="9"/>
+      <c r="B41" s="9"/>
+      <c r="C41" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="36.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A42" s="9"/>
+      <c r="B42" s="16"/>
+      <c r="C42" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="D40" s="5" t="s">
+      <c r="D42" s="6" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="120" x14ac:dyDescent="0.35">
-      <c r="A41" s="13"/>
-      <c r="B41" s="13"/>
-      <c r="C41" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="D41" s="5" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="96.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A42" s="13"/>
-      <c r="B42" s="15"/>
-      <c r="C42" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="D42" s="6" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="36.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A43" s="13"/>
+    <row r="43" spans="1:4" ht="24.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A43" s="9"/>
       <c r="B43" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C43" s="44" t="s">
+      <c r="C43" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="D43" s="45"/>
-    </row>
-    <row r="44" spans="1:4" ht="24.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A44" s="14"/>
+      <c r="D43" s="34"/>
+    </row>
+    <row r="44" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A44" s="10"/>
       <c r="B44" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C44" s="46" t="s">
+      <c r="C44" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="D44" s="47"/>
+      <c r="D44" s="22"/>
     </row>
     <row r="45" spans="1:4" ht="108" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A45" s="36" t="s">
+      <c r="A45" s="8" t="s">
         <v>55</v>
       </c>
       <c r="B45" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="C45" s="10" t="s">
+      <c r="C45" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="D45" s="11"/>
+      <c r="D45" s="20"/>
     </row>
     <row r="46" spans="1:4" ht="120" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A46" s="14"/>
+      <c r="A46" s="10"/>
       <c r="B46" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C46" s="46" t="s">
+      <c r="C46" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="D46" s="47"/>
+      <c r="D46" s="22"/>
     </row>
     <row r="47" spans="1:4" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A47" s="36" t="s">
+      <c r="A47" s="8" t="s">
         <v>60</v>
       </c>
       <c r="B47" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="C47" s="37" t="s">
+      <c r="C47" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="D47" s="38"/>
+      <c r="D47" s="12"/>
     </row>
     <row r="48" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A48" s="13"/>
+      <c r="A48" s="9"/>
       <c r="B48" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="C48" s="16" t="s">
+      <c r="C48" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="D48" s="17"/>
+      <c r="D48" s="14"/>
     </row>
     <row r="49" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A49" s="13"/>
+      <c r="A49" s="9"/>
       <c r="B49" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="C49" s="16" t="s">
+      <c r="C49" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="D49" s="17"/>
-    </row>
-    <row r="50" spans="1:4" ht="24.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A50" s="13"/>
+      <c r="D49" s="14"/>
+    </row>
+    <row r="50" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A50" s="9"/>
       <c r="B50" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="C50" s="16" t="s">
+      <c r="C50" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="D50" s="17"/>
-    </row>
-    <row r="51" spans="1:4" ht="24.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A51" s="13"/>
+      <c r="D50" s="14"/>
+    </row>
+    <row r="51" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A51" s="9"/>
       <c r="B51" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="C51" s="16" t="s">
+      <c r="C51" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="D51" s="17"/>
+      <c r="D51" s="14"/>
     </row>
     <row r="52" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A52" s="13"/>
-      <c r="B52" s="12" t="s">
+      <c r="A52" s="9"/>
+      <c r="B52" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="C52" s="16" t="s">
+      <c r="C52" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="D52" s="17"/>
+      <c r="D52" s="14"/>
     </row>
     <row r="53" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A53" s="13"/>
-      <c r="B53" s="15"/>
-      <c r="C53" s="16" t="s">
+      <c r="A53" s="9"/>
+      <c r="B53" s="16"/>
+      <c r="C53" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="D53" s="17"/>
+      <c r="D53" s="14"/>
     </row>
     <row r="54" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A54" s="14"/>
+      <c r="A54" s="10"/>
       <c r="B54" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C54" s="18" t="s">
+      <c r="C54" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="D54" s="19"/>
+      <c r="D54" s="24"/>
     </row>
     <row r="55" spans="1:4" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A55" s="36" t="s">
+      <c r="A55" s="8" t="s">
         <v>76</v>
       </c>
       <c r="B55" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="C55" s="37" t="s">
+      <c r="C55" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="D55" s="38"/>
-    </row>
-    <row r="56" spans="1:4" ht="36.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A56" s="13"/>
+      <c r="D55" s="12"/>
+    </row>
+    <row r="56" spans="1:4" ht="24.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A56" s="9"/>
       <c r="B56" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="C56" s="16" t="s">
+      <c r="C56" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="D56" s="17"/>
-    </row>
-    <row r="57" spans="1:4" ht="36.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A57" s="13"/>
+      <c r="D56" s="14"/>
+    </row>
+    <row r="57" spans="1:4" ht="24.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A57" s="9"/>
       <c r="B57" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="C57" s="16" t="s">
+      <c r="C57" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="D57" s="17"/>
+      <c r="D57" s="14"/>
     </row>
     <row r="58" spans="1:4" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A58" s="14"/>
+      <c r="A58" s="10"/>
       <c r="B58" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="C58" s="48" t="s">
+      <c r="C58" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="D58" s="49"/>
+      <c r="D58" s="32"/>
     </row>
     <row r="59" spans="1:4" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A59" s="36" t="s">
+      <c r="A59" s="8" t="s">
         <v>85</v>
       </c>
       <c r="B59" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="C59" s="37" t="s">
+      <c r="C59" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="D59" s="38"/>
-    </row>
-    <row r="60" spans="1:4" ht="24.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A60" s="13"/>
+      <c r="D59" s="12"/>
+    </row>
+    <row r="60" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A60" s="9"/>
       <c r="B60" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="C60" s="16" t="s">
+      <c r="C60" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="D60" s="17"/>
+      <c r="D60" s="14"/>
     </row>
     <row r="61" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A61" s="13"/>
+      <c r="A61" s="9"/>
       <c r="B61" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="C61" s="16" t="s">
+      <c r="C61" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="D61" s="17"/>
+      <c r="D61" s="14"/>
     </row>
     <row r="62" spans="1:4" ht="24.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A62" s="13"/>
+      <c r="A62" s="9"/>
       <c r="B62" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="C62" s="16" t="s">
+      <c r="C62" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="D62" s="17"/>
-    </row>
-    <row r="63" spans="1:4" ht="24.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A63" s="13"/>
+      <c r="D62" s="14"/>
+    </row>
+    <row r="63" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A63" s="9"/>
       <c r="B63" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="C63" s="16" t="s">
+      <c r="C63" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="D63" s="17"/>
+      <c r="D63" s="14"/>
     </row>
     <row r="64" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A64" s="14"/>
+      <c r="A64" s="10"/>
       <c r="B64" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="C64" s="18" t="s">
+      <c r="C64" s="23" t="s">
         <v>96</v>
       </c>
-      <c r="D64" s="19"/>
+      <c r="D64" s="24"/>
     </row>
     <row r="65" spans="1:4" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A65" s="36" t="s">
+      <c r="A65" s="8" t="s">
         <v>97</v>
       </c>
       <c r="B65" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="C65" s="37" t="s">
-        <v>134</v>
-      </c>
-      <c r="D65" s="38"/>
+      <c r="C65" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="D65" s="12"/>
     </row>
     <row r="66" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A66" s="14"/>
+      <c r="A66" s="10"/>
       <c r="B66" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="C66" s="18" t="s">
+      <c r="C66" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="D66" s="19"/>
+      <c r="D66" s="24"/>
     </row>
     <row r="67" spans="1:4" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A67" s="36" t="s">
+      <c r="A67" s="8" t="s">
         <v>101</v>
       </c>
       <c r="B67" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="C67" s="37" t="s">
+      <c r="C67" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="D67" s="38"/>
+      <c r="D67" s="12"/>
     </row>
     <row r="68" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A68" s="13"/>
-      <c r="B68" s="12" t="s">
+      <c r="A68" s="9"/>
+      <c r="B68" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="C68" s="16" t="s">
+      <c r="C68" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="D68" s="17"/>
+      <c r="D68" s="14"/>
     </row>
     <row r="69" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A69" s="13"/>
-      <c r="B69" s="15"/>
-      <c r="C69" s="16" t="s">
+      <c r="A69" s="9"/>
+      <c r="B69" s="16"/>
+      <c r="C69" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="D69" s="17"/>
+      <c r="D69" s="14"/>
     </row>
     <row r="70" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A70" s="13"/>
-      <c r="B70" s="12" t="s">
+      <c r="A70" s="9"/>
+      <c r="B70" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="C70" s="16" t="s">
+      <c r="C70" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="D70" s="17"/>
+      <c r="D70" s="14"/>
     </row>
     <row r="71" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A71" s="14"/>
-      <c r="B71" s="14"/>
-      <c r="C71" s="18" t="s">
+      <c r="A71" s="10"/>
+      <c r="B71" s="10"/>
+      <c r="C71" s="23" t="s">
         <v>109</v>
       </c>
-      <c r="D71" s="19"/>
-    </row>
-    <row r="72" spans="1:4" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A72" s="36" t="s">
+      <c r="D71" s="24"/>
+    </row>
+    <row r="72" spans="1:4" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A72" s="8" t="s">
         <v>110</v>
       </c>
       <c r="B72" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="C72" s="37" t="s">
+      <c r="C72" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="D72" s="38"/>
-    </row>
-    <row r="73" spans="1:4" ht="36.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A73" s="14"/>
+      <c r="D72" s="12"/>
+    </row>
+    <row r="73" spans="1:4" ht="24.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A73" s="10"/>
       <c r="B73" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="C73" s="18" t="s">
+      <c r="C73" s="23" t="s">
         <v>114</v>
       </c>
-      <c r="D73" s="19"/>
+      <c r="D73" s="24"/>
     </row>
     <row r="74" spans="1:4" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A74" s="30" t="s">
+      <c r="A74" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="B74" s="31"/>
-      <c r="C74" s="37" t="s">
+      <c r="B74" s="26"/>
+      <c r="C74" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="D74" s="38"/>
+      <c r="D74" s="12"/>
     </row>
     <row r="75" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A75" s="32"/>
-      <c r="B75" s="33"/>
-      <c r="C75" s="16" t="s">
+      <c r="A75" s="27"/>
+      <c r="B75" s="28"/>
+      <c r="C75" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="D75" s="17"/>
+      <c r="D75" s="14"/>
     </row>
     <row r="76" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A76" s="50"/>
-      <c r="B76" s="51"/>
-      <c r="C76" s="18" t="s">
+      <c r="A76" s="29"/>
+      <c r="B76" s="30"/>
+      <c r="C76" s="23" t="s">
         <v>118</v>
       </c>
-      <c r="D76" s="19"/>
+      <c r="D76" s="24"/>
     </row>
     <row r="77" spans="1:4" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A77" s="30" t="s">
+      <c r="A77" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="B77" s="31"/>
-      <c r="C77" s="37" t="s">
+      <c r="B77" s="26"/>
+      <c r="C77" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="D77" s="38"/>
+      <c r="D77" s="12"/>
     </row>
     <row r="78" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A78" s="32"/>
-      <c r="B78" s="33"/>
-      <c r="C78" s="16" t="s">
+      <c r="A78" s="27"/>
+      <c r="B78" s="28"/>
+      <c r="C78" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="D78" s="17"/>
+      <c r="D78" s="14"/>
     </row>
     <row r="79" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A79" s="32"/>
-      <c r="B79" s="33"/>
-      <c r="C79" s="16" t="s">
+      <c r="A79" s="27"/>
+      <c r="B79" s="28"/>
+      <c r="C79" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="D79" s="17"/>
+      <c r="D79" s="14"/>
     </row>
     <row r="80" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A80" s="32"/>
-      <c r="B80" s="33"/>
-      <c r="C80" s="16" t="s">
+      <c r="A80" s="27"/>
+      <c r="B80" s="28"/>
+      <c r="C80" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="D80" s="17"/>
+      <c r="D80" s="14"/>
     </row>
     <row r="81" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A81" s="50"/>
-      <c r="B81" s="51"/>
-      <c r="C81" s="18" t="s">
+      <c r="A81" s="29"/>
+      <c r="B81" s="30"/>
+      <c r="C81" s="23" t="s">
         <v>124</v>
       </c>
-      <c r="D81" s="19"/>
+      <c r="D81" s="24"/>
     </row>
     <row r="82" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="90">
-    <mergeCell ref="A47:A54"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="C51:D51"/>
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="C52:D52"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="B40:B42"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="C81:D81"/>
-    <mergeCell ref="C78:D78"/>
-    <mergeCell ref="C79:D79"/>
-    <mergeCell ref="C80:D80"/>
-    <mergeCell ref="A77:B81"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:A9"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="A12:B14"/>
+    <mergeCell ref="A15:A21"/>
+    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="A22:A29"/>
+    <mergeCell ref="B25:B27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="A30:A36"/>
+    <mergeCell ref="B31:B33"/>
+    <mergeCell ref="D31:D33"/>
+    <mergeCell ref="B34:B36"/>
+    <mergeCell ref="A37:A44"/>
+    <mergeCell ref="A55:A58"/>
+    <mergeCell ref="A59:A64"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="C60:D60"/>
+    <mergeCell ref="C61:D61"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="C63:D63"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="C56:D56"/>
+    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="C58:D58"/>
+    <mergeCell ref="C59:D59"/>
+    <mergeCell ref="C65:D65"/>
+    <mergeCell ref="C66:D66"/>
+    <mergeCell ref="C67:D67"/>
+    <mergeCell ref="C68:D68"/>
+    <mergeCell ref="A65:A66"/>
     <mergeCell ref="C75:D75"/>
     <mergeCell ref="C76:D76"/>
     <mergeCell ref="C77:D77"/>
@@ -2811,62 +2847,26 @@
     <mergeCell ref="B68:B69"/>
     <mergeCell ref="B70:B71"/>
     <mergeCell ref="A72:A73"/>
-    <mergeCell ref="C65:D65"/>
-    <mergeCell ref="C66:D66"/>
-    <mergeCell ref="C67:D67"/>
-    <mergeCell ref="C68:D68"/>
-    <mergeCell ref="A65:A66"/>
-    <mergeCell ref="C55:D55"/>
-    <mergeCell ref="C56:D56"/>
-    <mergeCell ref="C57:D57"/>
-    <mergeCell ref="C58:D58"/>
-    <mergeCell ref="C59:D59"/>
-    <mergeCell ref="C60:D60"/>
-    <mergeCell ref="C61:D61"/>
-    <mergeCell ref="C62:D62"/>
-    <mergeCell ref="C63:D63"/>
-    <mergeCell ref="C64:D64"/>
-    <mergeCell ref="A55:A58"/>
-    <mergeCell ref="A59:A64"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="C53:D53"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="A30:A36"/>
-    <mergeCell ref="B31:B33"/>
-    <mergeCell ref="D31:D33"/>
-    <mergeCell ref="B34:B36"/>
-    <mergeCell ref="A37:A44"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="A22:A29"/>
-    <mergeCell ref="B25:B27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="A12:B14"/>
-    <mergeCell ref="A15:A21"/>
-    <mergeCell ref="B16:B18"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:A9"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C81:D81"/>
+    <mergeCell ref="C78:D78"/>
+    <mergeCell ref="C79:D79"/>
+    <mergeCell ref="C80:D80"/>
+    <mergeCell ref="A77:B81"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="B40:B42"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="A47:A54"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="C52:D52"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>